<commit_message>
add changes to Data xlsx
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -14,57 +14,63 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>Months</t>
   </si>
   <si>
+    <t>Monthly sales</t>
+  </si>
+  <si>
+    <t>% of change sales</t>
+  </si>
+  <si>
+    <t>Minimum Sales</t>
+  </si>
+  <si>
+    <t>Max Sales</t>
+  </si>
+  <si>
+    <t>Jan</t>
+  </si>
+  <si>
+    <t>Feb</t>
+  </si>
+  <si>
+    <t>March</t>
+  </si>
+  <si>
+    <t>April</t>
+  </si>
+  <si>
+    <t>May</t>
+  </si>
+  <si>
+    <t>June</t>
+  </si>
+  <si>
+    <t>July</t>
+  </si>
+  <si>
+    <t>August</t>
+  </si>
+  <si>
+    <t>September</t>
+  </si>
+  <si>
+    <t>October</t>
+  </si>
+  <si>
+    <t>Nov</t>
+  </si>
+  <si>
+    <t>Dec</t>
+  </si>
+  <si>
+    <t>Total Sales</t>
+  </si>
+  <si>
     <t>Average Sales</t>
-  </si>
-  <si>
-    <t>Minimum Sales</t>
-  </si>
-  <si>
-    <t>Max Sales</t>
-  </si>
-  <si>
-    <t>Total Sales</t>
-  </si>
-  <si>
-    <t>Jan</t>
-  </si>
-  <si>
-    <t>Feb</t>
-  </si>
-  <si>
-    <t>March</t>
-  </si>
-  <si>
-    <t>April</t>
-  </si>
-  <si>
-    <t>May</t>
-  </si>
-  <si>
-    <t>June</t>
-  </si>
-  <si>
-    <t>July</t>
-  </si>
-  <si>
-    <t>August</t>
-  </si>
-  <si>
-    <t>September</t>
-  </si>
-  <si>
-    <t>October</t>
-  </si>
-  <si>
-    <t>Nov</t>
-  </si>
-  <si>
-    <t>Dec</t>
   </si>
 </sst>
 </file>
@@ -396,7 +402,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -489,6 +495,16 @@
         <v>16</v>
       </c>
     </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>